<commit_message>
Changed LED nominal, and general cleanup
</commit_message>
<xml_diff>
--- a/Bill of Materials-MR-SP3SM_r1.xlsx
+++ b/Bill of Materials-MR-SP3SM_r1.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="91">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="90">
   <si>
     <t>Designator</t>
   </si>
@@ -216,22 +216,19 @@
     <t>R7, R8, R9</t>
   </si>
   <si>
-    <t>R_0603_6800</t>
-  </si>
-  <si>
-    <t>6.8k</t>
-  </si>
-  <si>
-    <t>Resistor 0603 6.8k 1/10W</t>
+    <t>R_0603_10000</t>
+  </si>
+  <si>
+    <t>10k</t>
+  </si>
+  <si>
+    <t>Resistor 0603 10k 1/10W</t>
   </si>
   <si>
     <t>R10, R11, R12, R13, R14, R15, R19, R20, R25, R26, R28, R29</t>
   </si>
   <si>
     <t>R_0402_10000</t>
-  </si>
-  <si>
-    <t>10k</t>
   </si>
   <si>
     <t>Resistor 0402 10k 1/16W</t>
@@ -648,16 +645,16 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="18" customWidth="1"/>
-    <col min="2" max="2" width="12" customWidth="1"/>
-    <col min="3" max="3" width="20.5703125" customWidth="1"/>
-    <col min="4" max="4" width="26.5703125" customWidth="1"/>
-    <col min="5" max="5" width="13.7109375" customWidth="1"/>
-    <col min="6" max="6" width="40.28515625" customWidth="1"/>
-    <col min="7" max="7" width="22.7109375" customWidth="1"/>
-    <col min="8" max="8" width="16" customWidth="1"/>
-    <col min="9" max="9" width="9.85546875" customWidth="1"/>
-    <col min="10" max="10" width="8.5703125" customWidth="1"/>
+    <col min="1" max="1" width="43.42578125" customWidth="1"/>
+    <col min="2" max="2" width="7.28515625" customWidth="1"/>
+    <col min="3" max="3" width="17.28515625" customWidth="1"/>
+    <col min="4" max="4" width="15.140625" customWidth="1"/>
+    <col min="5" max="5" width="11.7109375" customWidth="1"/>
+    <col min="6" max="6" width="36" customWidth="1"/>
+    <col min="7" max="7" width="13.42578125" customWidth="1"/>
+    <col min="8" max="8" width="7.42578125" customWidth="1"/>
+    <col min="9" max="9" width="8.140625" customWidth="1"/>
+    <col min="10" max="10" width="26.85546875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
@@ -1087,16 +1084,16 @@
         <v>69</v>
       </c>
       <c r="D14" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="E14" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F14" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="E14" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F14" s="2" t="s">
+      <c r="G14" s="2" t="s">
         <v>71</v>
-      </c>
-      <c r="G14" s="2" t="s">
-        <v>72</v>
       </c>
       <c r="H14" s="3">
         <v>12</v>
@@ -1110,22 +1107,22 @@
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B15" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C15" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="B15" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C15" s="2" t="s">
+      <c r="D15" s="2" t="s">
         <v>74</v>
       </c>
-      <c r="D15" s="2" t="s">
+      <c r="E15" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F15" s="2" t="s">
         <v>75</v>
-      </c>
-      <c r="E15" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F15" s="2" t="s">
-        <v>76</v>
       </c>
       <c r="G15" s="2" t="s">
         <v>62</v>
@@ -1142,31 +1139,31 @@
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
+        <v>76</v>
+      </c>
+      <c r="B16" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C16" s="2" t="s">
         <v>77</v>
       </c>
-      <c r="B16" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C16" s="2" t="s">
+      <c r="D16" s="2" t="s">
         <v>78</v>
       </c>
-      <c r="D16" s="2" t="s">
+      <c r="E16" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F16" s="2" t="s">
         <v>79</v>
       </c>
-      <c r="E16" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F16" s="2" t="s">
-        <v>80</v>
-      </c>
       <c r="G16" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H16" s="3">
         <v>2</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="J16" s="2" t="s">
         <v>11</v>
@@ -1174,7 +1171,7 @@
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>11</v>
@@ -1183,22 +1180,22 @@
         <v>69</v>
       </c>
       <c r="D17" s="2" t="s">
+        <v>66</v>
+      </c>
+      <c r="E17" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F17" s="2" t="s">
         <v>70</v>
       </c>
-      <c r="E17" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F17" s="2" t="s">
+      <c r="G17" s="2" t="s">
         <v>71</v>
-      </c>
-      <c r="G17" s="2" t="s">
-        <v>72</v>
       </c>
       <c r="H17" s="3">
         <v>1</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="J17" s="2" t="s">
         <v>11</v>
@@ -1206,31 +1203,31 @@
     </row>
     <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
+        <v>82</v>
+      </c>
+      <c r="B18" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C18" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="B18" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C18" s="2" t="s">
+      <c r="D18" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="D18" s="2" t="s">
+      <c r="E18" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="F18" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="E18" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="F18" s="2" t="s">
-        <v>86</v>
-      </c>
       <c r="G18" s="2" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="H18" s="3">
         <v>1</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="J18" s="2" t="s">
         <v>11</v>
@@ -1238,25 +1235,25 @@
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
+        <v>86</v>
+      </c>
+      <c r="B19" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C19" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="B19" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C19" s="2" t="s">
+      <c r="D19" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="D19" s="2" t="s">
+      <c r="E19" s="2" t="s">
+        <v>87</v>
+      </c>
+      <c r="F19" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="E19" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="F19" s="2" t="s">
-        <v>90</v>
-      </c>
       <c r="G19" s="2" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="H19" s="3">
         <v>3</v>

</xml_diff>